<commit_message>
tela inicial pre feita
</commit_message>
<xml_diff>
--- a/Estrutura_de_equipamentos.xlsx
+++ b/Estrutura_de_equipamentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitcold.sharepoint.com/sites/ti/Shared Documents/PROJETO_PADRAO_MAQUINAS_UNITCOLD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="11_A1DB469C4DC833DA4CF098B7DA0E6B1B3ED6D1EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EDAFF11-807E-43FC-A05A-1C60D2747EC9}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="11_A1DB469C4DC833DA4CF098B7DA0E6B1B3ED6D1EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2EA4F39-AE95-4B2C-BF1C-612FA32BBA19}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>CR-FTC</t>
   </si>
@@ -180,6 +180,24 @@
   </si>
   <si>
     <t>xR</t>
+  </si>
+  <si>
+    <t>0,75 TR</t>
+  </si>
+  <si>
+    <t>1,00 TR</t>
+  </si>
+  <si>
+    <t>1,50 TR</t>
+  </si>
+  <si>
+    <t>2,00 TR</t>
+  </si>
+  <si>
+    <t>2,50 TR</t>
+  </si>
+  <si>
+    <t>3,00 TR</t>
   </si>
 </sst>
 </file>
@@ -218,14 +236,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -513,12 +528,12 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="8.88671875" style="3"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -609,8 +624,8 @@
         <f t="shared" si="0"/>
         <v>007-2</v>
       </c>
-      <c r="E5" s="2">
-        <v>0.75</v>
+      <c r="E5" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -627,8 +642,8 @@
         <f t="shared" si="0"/>
         <v>010-2</v>
       </c>
-      <c r="E6" s="2">
-        <v>1</v>
+      <c r="E6" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -645,8 +660,8 @@
         <f t="shared" si="0"/>
         <v>015-2</v>
       </c>
-      <c r="E7" s="2">
-        <v>1.5</v>
+      <c r="E7" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -663,8 +678,8 @@
         <f t="shared" si="0"/>
         <v>020-2</v>
       </c>
-      <c r="E8" s="2">
-        <v>2</v>
+      <c r="E8" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -681,8 +696,8 @@
         <f t="shared" si="0"/>
         <v>025-2</v>
       </c>
-      <c r="E9" s="2">
-        <v>2.5</v>
+      <c r="E9" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -699,8 +714,8 @@
         <f t="shared" si="0"/>
         <v>030-2</v>
       </c>
-      <c r="E10" s="2">
-        <v>3</v>
+      <c r="E10" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -962,21 +977,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010011CE1B6871DF5745999C1E7BF1D3C675" ma:contentTypeVersion="3" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="4671a090984673c98d9f3d802cfbd84b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c754d3dd-89a9-458c-b6b9-d71350aaa213" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bff7ac9043df59347ee870742dd3d242" ns2:_="">
     <xsd:import namespace="c754d3dd-89a9-458c-b6b9-d71350aaa213"/>
@@ -1114,24 +1114,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FED4FE8-8227-40E8-8088-9DE0F3FBFB99}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB94E07A-902E-4024-9403-0B9E53B2B275}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEBE209C-7BB1-4667-8BA2-62EC8B82B4C7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1147,4 +1145,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB94E07A-902E-4024-9403-0B9E53B2B275}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FED4FE8-8227-40E8-8088-9DE0F3FBFB99}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
incluido todas opções de maquinas que temos e selecoes possiveis
</commit_message>
<xml_diff>
--- a/Estrutura_de_equipamentos.xlsx
+++ b/Estrutura_de_equipamentos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitcold.sharepoint.com/sites/ti/Shared Documents/PROJETO_PADRAO_MAQUINAS_UNITCOLD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="11_A1DB469C4DC833DA4CF098B7DA0E6B1B3ED6D1EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2EA4F39-AE95-4B2C-BF1C-612FA32BBA19}"/>
+  <xr:revisionPtr revIDLastSave="462" documentId="11_A1DB469C4DC833DA4CF098B7DA0E6B1B3ED6D1EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4C14695-94C2-49B6-B9FB-5AAD42C07D14}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fancoletes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="144">
   <si>
     <t>CR-FTC</t>
   </si>
@@ -198,6 +198,276 @@
   </si>
   <si>
     <t>3,00 TR</t>
+  </si>
+  <si>
+    <t>CR-UTV</t>
+  </si>
+  <si>
+    <t>Unidade de tratamento de ar vertical</t>
+  </si>
+  <si>
+    <t>040</t>
+  </si>
+  <si>
+    <t>050</t>
+  </si>
+  <si>
+    <t>075</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>4,00 TR</t>
+  </si>
+  <si>
+    <t>5,00 TR</t>
+  </si>
+  <si>
+    <t>7,50 TR</t>
+  </si>
+  <si>
+    <t>10,00 TR</t>
+  </si>
+  <si>
+    <t>15,00 TR</t>
+  </si>
+  <si>
+    <t>20,00 TR</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Configuração Superior (25mm com thermalbreak)</t>
+  </si>
+  <si>
+    <t>Configuração Premium (45mm com thermalbreak)</t>
+  </si>
+  <si>
+    <t>CR-UTA</t>
+  </si>
+  <si>
+    <t>Unidade de tratamento de ar</t>
+  </si>
+  <si>
+    <t>0510</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>1510</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>DD-S</t>
+  </si>
+  <si>
+    <t>DD-P</t>
+  </si>
+  <si>
+    <t>Configuração Duplo Deck com perfil superior (25mm com thermalbreak)</t>
+  </si>
+  <si>
+    <t>Configuração Duplo Deck com perfil premium (45mm com thermalbreak)</t>
+  </si>
+  <si>
+    <t>LL</t>
+  </si>
+  <si>
+    <t>PF</t>
+  </si>
+  <si>
+    <t>Ventilador Limit Load</t>
+  </si>
+  <si>
+    <t>Radial plenum fan com motor AC</t>
+  </si>
+  <si>
+    <t>CF-AHU</t>
+  </si>
+  <si>
+    <t>Air Handler Conforto</t>
+  </si>
+  <si>
+    <t>CC-AHU</t>
+  </si>
+  <si>
+    <t>Air Handler de Precisão</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>027</t>
+  </si>
+  <si>
+    <t>034</t>
+  </si>
+  <si>
+    <t>051</t>
+  </si>
+  <si>
+    <t>068</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>204</t>
+  </si>
+  <si>
+    <t>238</t>
+  </si>
+  <si>
+    <t>272</t>
+  </si>
+  <si>
+    <t>306</t>
+  </si>
+  <si>
+    <t>340</t>
+  </si>
+  <si>
+    <t>408</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Configuração perfil padrão 25mm</t>
+  </si>
+  <si>
+    <t>Ventilador sirocco</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>G4+M5 ou G4+F8</t>
+  </si>
+  <si>
+    <t>1 estágio de filtragem antes do ventilador</t>
+  </si>
+  <si>
+    <t>2 estágios de filtragem antes do ventilador</t>
+  </si>
+  <si>
+    <t>Modelo (Vazão nominal em m³/h / 1000)</t>
+  </si>
+  <si>
+    <t>Configuração do Gabinete</t>
+  </si>
+  <si>
+    <t>Acessórios</t>
+  </si>
+  <si>
+    <t>Modelo (Matriz de filtragem)</t>
+  </si>
+  <si>
+    <t>fancoletes</t>
+  </si>
+  <si>
+    <t>unid_tratamento_ar_v</t>
+  </si>
+  <si>
+    <t>Largura = 1/2 elemento (289mm) + Altura = 1 elemento (595mm)</t>
+  </si>
+  <si>
+    <t>Largura = 1 elemento (595mm) + Altura = 1 elemento (595mm)</t>
+  </si>
+  <si>
+    <t>Largura = 1 elemento (595mm) + 1/2 elemento (289mm) + Altura = 1 elemento (595mm)</t>
+  </si>
+  <si>
+    <t>Largura = 2 elementos (595mm) + Altura = 1 elemento (595mm)</t>
+  </si>
+  <si>
+    <t>Largura = 2 elementos (595mm) + Altura = 1 elemento (595mm) + 1/2 elemento (289mm)</t>
+  </si>
+  <si>
+    <t>Largura = 2 elementos (595mm) + Altura = 2 elementos (595mm)</t>
+  </si>
+  <si>
+    <t>unid_tratamento_ar</t>
+  </si>
+  <si>
+    <t>1,00 TR-680 m³/h</t>
+  </si>
+  <si>
+    <t>2,00 TR-1.360 m³/h</t>
+  </si>
+  <si>
+    <t>3,00 TR-2.040 m³/h</t>
+  </si>
+  <si>
+    <t>4,00 TR-2.720 m³/h</t>
+  </si>
+  <si>
+    <t>5,00 TR-3.400 m³/h</t>
+  </si>
+  <si>
+    <t>7,50 TR-5.100 m³/h</t>
+  </si>
+  <si>
+    <t>10,00 TR-6.800 m³/h</t>
+  </si>
+  <si>
+    <t>15,00 TR-10.200 m³/h</t>
+  </si>
+  <si>
+    <t>20,00 TR-13.600 m³/h</t>
+  </si>
+  <si>
+    <t>25,00 TR-17.000 m³/h</t>
+  </si>
+  <si>
+    <t>30,00 TR-20.400 m³/h</t>
+  </si>
+  <si>
+    <t>35,00 TR-23.800 m³/h</t>
+  </si>
+  <si>
+    <t>40,00 TR-27.200 m³/h</t>
+  </si>
+  <si>
+    <t>45,00 TR-30.600 m³/h</t>
+  </si>
+  <si>
+    <t>50,00 TR-34.000 m³/h</t>
+  </si>
+  <si>
+    <t>60,00 TR-40.800 m³/h</t>
+  </si>
+  <si>
+    <t>air_handler</t>
   </si>
 </sst>
 </file>
@@ -525,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,9 +806,10 @@
     <col min="2" max="2" width="8.88671875" style="3"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -555,8 +826,11 @@
       <c r="E1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -567,14 +841,17 @@
         <v>39</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D24" si="0">A2&amp;"-"&amp;B2</f>
+        <f t="shared" ref="D2:D65" si="0">A2&amp;"-"&amp;B2</f>
         <v>CR-FTH-1</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -591,8 +868,11 @@
       <c r="E3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -609,8 +889,11 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -627,8 +910,11 @@
       <c r="E5" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -645,8 +931,11 @@
       <c r="E6" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -663,8 +952,11 @@
       <c r="E7" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -681,8 +973,11 @@
       <c r="E8" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -699,8 +994,11 @@
       <c r="E9" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -717,8 +1015,11 @@
       <c r="E10" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -735,8 +1036,11 @@
       <c r="E11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -753,8 +1057,11 @@
       <c r="E12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -771,8 +1078,11 @@
       <c r="E13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -789,8 +1099,11 @@
       <c r="E14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -807,8 +1120,11 @@
       <c r="E15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -825,8 +1141,11 @@
       <c r="E16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -843,8 +1162,11 @@
       <c r="E17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -861,8 +1183,11 @@
       <c r="E18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -879,8 +1204,11 @@
       <c r="E19" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -897,8 +1225,11 @@
       <c r="E20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -915,8 +1246,11 @@
       <c r="E21" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -933,8 +1267,11 @@
       <c r="E22" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -951,8 +1288,11 @@
       <c r="E23" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -969,14 +1309,2021 @@
       <c r="E24" t="s">
         <v>38</v>
       </c>
+      <c r="F24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>CR-UTV-1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>010-2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="3">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>020-2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="3">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>030-2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="3">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>040-2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="3">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>050-2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="3">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>075-2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>100-2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="3">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>150-2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="3">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>200-2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="3">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>S-3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="3">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>P-3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="3">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>x/x-4</v>
+      </c>
+      <c r="E37" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="3">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>xR-4</v>
+      </c>
+      <c r="E38" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="3">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>SS-5</v>
+      </c>
+      <c r="E39" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="3">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>TN-5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>21</v>
+      </c>
+      <c r="F40" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="3">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>DK-5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>22</v>
+      </c>
+      <c r="F41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="3">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>LG-5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="3">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>EC-6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="3">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>G4 / M5 ou G4+M5-7</v>
+      </c>
+      <c r="E44" t="s">
+        <v>30</v>
+      </c>
+      <c r="F44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="3">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>G4+F9-7</v>
+      </c>
+      <c r="E45" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" s="3">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>G4+F9+H14-7</v>
+      </c>
+      <c r="E46" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="3">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>Acessorios-8</v>
+      </c>
+      <c r="E47" t="s">
+        <v>35</v>
+      </c>
+      <c r="F47" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="3">
+        <v>9</v>
+      </c>
+      <c r="C48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>X-9</v>
+      </c>
+      <c r="E48" t="s">
+        <v>37</v>
+      </c>
+      <c r="F48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" s="3">
+        <v>9</v>
+      </c>
+      <c r="C49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>E -9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F49" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50" s="3">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>CR-UTA-1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>73</v>
+      </c>
+      <c r="F50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="3">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>117</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>0510-2</v>
+      </c>
+      <c r="E51" t="s">
+        <v>120</v>
+      </c>
+      <c r="F51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="3">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>117</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>1010-2</v>
+      </c>
+      <c r="E52" t="s">
+        <v>121</v>
+      </c>
+      <c r="F52" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" s="3">
+        <v>2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>117</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>1510-2</v>
+      </c>
+      <c r="E53" t="s">
+        <v>122</v>
+      </c>
+      <c r="F53" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" s="3">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>117</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>2010-2</v>
+      </c>
+      <c r="E54" t="s">
+        <v>123</v>
+      </c>
+      <c r="F54" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55" s="3">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>117</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>2015-2</v>
+      </c>
+      <c r="E55" t="s">
+        <v>124</v>
+      </c>
+      <c r="F55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>79</v>
+      </c>
+      <c r="B56" s="3">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>2020-2</v>
+      </c>
+      <c r="E56" t="s">
+        <v>125</v>
+      </c>
+      <c r="F56" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>2520</v>
+      </c>
+      <c r="B57" s="3">
+        <v>2</v>
+      </c>
+      <c r="C57" t="s">
+        <v>117</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>2520-2</v>
+      </c>
+      <c r="F57" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>2540</v>
+      </c>
+      <c r="B58" s="3">
+        <v>2</v>
+      </c>
+      <c r="C58" t="s">
+        <v>117</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>2540-2</v>
+      </c>
+      <c r="F58" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>3020</v>
+      </c>
+      <c r="B59" s="3">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>117</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>3020-2</v>
+      </c>
+      <c r="F59" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>3025</v>
+      </c>
+      <c r="B60" s="3">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>117</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>3025-2</v>
+      </c>
+      <c r="F60" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>3030</v>
+      </c>
+      <c r="B61" s="3">
+        <v>2</v>
+      </c>
+      <c r="C61" t="s">
+        <v>117</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>3030-2</v>
+      </c>
+      <c r="F61" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>3035</v>
+      </c>
+      <c r="B62" s="3">
+        <v>2</v>
+      </c>
+      <c r="C62" t="s">
+        <v>117</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>3035-2</v>
+      </c>
+      <c r="F62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>3530</v>
+      </c>
+      <c r="B63" s="3">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
+        <v>117</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v>3530-2</v>
+      </c>
+      <c r="F63" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>4030</v>
+      </c>
+      <c r="B64" s="3">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
+        <v>117</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v>4030-2</v>
+      </c>
+      <c r="F64" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>4530</v>
+      </c>
+      <c r="B65" s="3">
+        <v>2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>117</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v>4530-2</v>
+      </c>
+      <c r="F65" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="3">
+        <v>3</v>
+      </c>
+      <c r="C66" t="s">
+        <v>115</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" ref="D66:D120" si="1">A66&amp;"-"&amp;B66</f>
+        <v>S-3</v>
+      </c>
+      <c r="E66" t="s">
+        <v>70</v>
+      </c>
+      <c r="F66" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" s="3">
+        <v>3</v>
+      </c>
+      <c r="C67" t="s">
+        <v>115</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="1"/>
+        <v>P-3</v>
+      </c>
+      <c r="E67" t="s">
+        <v>71</v>
+      </c>
+      <c r="F67" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68" s="3">
+        <v>3</v>
+      </c>
+      <c r="C68" t="s">
+        <v>115</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="1"/>
+        <v>DD-S-3</v>
+      </c>
+      <c r="E68" t="s">
+        <v>82</v>
+      </c>
+      <c r="F68" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69" s="3">
+        <v>3</v>
+      </c>
+      <c r="C69" t="s">
+        <v>115</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="1"/>
+        <v>DD-P-3</v>
+      </c>
+      <c r="E69" t="s">
+        <v>83</v>
+      </c>
+      <c r="F69" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B70" s="3">
+        <v>4</v>
+      </c>
+      <c r="C70" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="1"/>
+        <v>x/x-4</v>
+      </c>
+      <c r="E70" t="s">
+        <v>18</v>
+      </c>
+      <c r="F70" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>47</v>
+      </c>
+      <c r="B71" s="3">
+        <v>4</v>
+      </c>
+      <c r="C71" t="s">
+        <v>41</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="1"/>
+        <v>xR-4</v>
+      </c>
+      <c r="E71" t="s">
+        <v>19</v>
+      </c>
+      <c r="F71" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" s="3">
+        <v>5</v>
+      </c>
+      <c r="C72" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="1"/>
+        <v>SS-5</v>
+      </c>
+      <c r="E72" t="s">
+        <v>20</v>
+      </c>
+      <c r="F72" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>11</v>
+      </c>
+      <c r="B73" s="3">
+        <v>5</v>
+      </c>
+      <c r="C73" t="s">
+        <v>42</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="1"/>
+        <v>TN-5</v>
+      </c>
+      <c r="E73" t="s">
+        <v>21</v>
+      </c>
+      <c r="F73" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>12</v>
+      </c>
+      <c r="B74" s="3">
+        <v>5</v>
+      </c>
+      <c r="C74" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="1"/>
+        <v>DK-5</v>
+      </c>
+      <c r="E74" t="s">
+        <v>22</v>
+      </c>
+      <c r="F74" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" s="3">
+        <v>5</v>
+      </c>
+      <c r="C75" t="s">
+        <v>42</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="1"/>
+        <v>LG-5</v>
+      </c>
+      <c r="E75" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>84</v>
+      </c>
+      <c r="B76" s="3">
+        <v>6</v>
+      </c>
+      <c r="C76" t="s">
+        <v>43</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="1"/>
+        <v>LL-6</v>
+      </c>
+      <c r="E76" t="s">
+        <v>86</v>
+      </c>
+      <c r="F76" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>85</v>
+      </c>
+      <c r="B77" s="3">
+        <v>6</v>
+      </c>
+      <c r="C77" t="s">
+        <v>43</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="1"/>
+        <v>PF-6</v>
+      </c>
+      <c r="E77" t="s">
+        <v>87</v>
+      </c>
+      <c r="F77" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>23</v>
+      </c>
+      <c r="B78" s="3">
+        <v>6</v>
+      </c>
+      <c r="C78" t="s">
+        <v>43</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="1"/>
+        <v>EC-6</v>
+      </c>
+      <c r="E78" t="s">
+        <v>25</v>
+      </c>
+      <c r="F78" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>27</v>
+      </c>
+      <c r="B79" s="3">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s">
+        <v>44</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="1"/>
+        <v>G4 / M5 ou G4+M5-7</v>
+      </c>
+      <c r="E79" t="s">
+        <v>30</v>
+      </c>
+      <c r="F79" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>28</v>
+      </c>
+      <c r="B80" s="3">
+        <v>7</v>
+      </c>
+      <c r="C80" t="s">
+        <v>44</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="1"/>
+        <v>G4+F9-7</v>
+      </c>
+      <c r="E80" t="s">
+        <v>31</v>
+      </c>
+      <c r="F80" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>29</v>
+      </c>
+      <c r="B81" s="3">
+        <v>7</v>
+      </c>
+      <c r="C81" t="s">
+        <v>44</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="1"/>
+        <v>G4+F9+H14-7</v>
+      </c>
+      <c r="E81" t="s">
+        <v>32</v>
+      </c>
+      <c r="F81" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>33</v>
+      </c>
+      <c r="B82" s="3">
+        <v>8</v>
+      </c>
+      <c r="C82" t="s">
+        <v>116</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="1"/>
+        <v>Acessorios-8</v>
+      </c>
+      <c r="E82" t="s">
+        <v>35</v>
+      </c>
+      <c r="F82" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>34</v>
+      </c>
+      <c r="B83" s="3">
+        <v>9</v>
+      </c>
+      <c r="C83" t="s">
+        <v>45</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="1"/>
+        <v>X-9</v>
+      </c>
+      <c r="E83" t="s">
+        <v>37</v>
+      </c>
+      <c r="F83" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>36</v>
+      </c>
+      <c r="B84" s="3">
+        <v>9</v>
+      </c>
+      <c r="C84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="1"/>
+        <v>E -9</v>
+      </c>
+      <c r="E84" t="s">
+        <v>38</v>
+      </c>
+      <c r="F84" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85" s="3">
+        <v>1</v>
+      </c>
+      <c r="C85" t="s">
+        <v>39</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="1"/>
+        <v>CF-AHU-1</v>
+      </c>
+      <c r="E85" t="s">
+        <v>89</v>
+      </c>
+      <c r="F85" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>90</v>
+      </c>
+      <c r="B86" s="3">
+        <v>1</v>
+      </c>
+      <c r="C86" t="s">
+        <v>39</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="1"/>
+        <v>CC-AHU-1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>91</v>
+      </c>
+      <c r="F86" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>92</v>
+      </c>
+      <c r="B87" s="3">
+        <v>2</v>
+      </c>
+      <c r="C87" t="s">
+        <v>114</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="1"/>
+        <v>006-2</v>
+      </c>
+      <c r="E87" t="s">
+        <v>127</v>
+      </c>
+      <c r="F87" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>93</v>
+      </c>
+      <c r="B88" s="3">
+        <v>2</v>
+      </c>
+      <c r="C88" t="s">
+        <v>114</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="1"/>
+        <v>013-2</v>
+      </c>
+      <c r="E88" t="s">
+        <v>128</v>
+      </c>
+      <c r="F88" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>7</v>
+      </c>
+      <c r="B89" s="3">
+        <v>2</v>
+      </c>
+      <c r="C89" t="s">
+        <v>114</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="1"/>
+        <v>020-2</v>
+      </c>
+      <c r="E89" t="s">
+        <v>129</v>
+      </c>
+      <c r="F89" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90" s="3">
+        <v>2</v>
+      </c>
+      <c r="C90" t="s">
+        <v>114</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="1"/>
+        <v>027-2</v>
+      </c>
+      <c r="E90" t="s">
+        <v>130</v>
+      </c>
+      <c r="F90" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>95</v>
+      </c>
+      <c r="B91" s="3">
+        <v>2</v>
+      </c>
+      <c r="C91" t="s">
+        <v>114</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="1"/>
+        <v>034-2</v>
+      </c>
+      <c r="E91" t="s">
+        <v>131</v>
+      </c>
+      <c r="F91" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92" s="3">
+        <v>2</v>
+      </c>
+      <c r="C92" t="s">
+        <v>114</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="1"/>
+        <v>051-2</v>
+      </c>
+      <c r="E92" t="s">
+        <v>132</v>
+      </c>
+      <c r="F92" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>97</v>
+      </c>
+      <c r="B93" s="3">
+        <v>2</v>
+      </c>
+      <c r="C93" t="s">
+        <v>114</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="1"/>
+        <v>068-2</v>
+      </c>
+      <c r="E93" t="s">
+        <v>133</v>
+      </c>
+      <c r="F93" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>98</v>
+      </c>
+      <c r="B94" s="3">
+        <v>2</v>
+      </c>
+      <c r="C94" t="s">
+        <v>114</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="1"/>
+        <v>102-2</v>
+      </c>
+      <c r="E94" t="s">
+        <v>134</v>
+      </c>
+      <c r="F94" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>99</v>
+      </c>
+      <c r="B95" s="3">
+        <v>2</v>
+      </c>
+      <c r="C95" t="s">
+        <v>114</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="1"/>
+        <v>136-2</v>
+      </c>
+      <c r="E95" t="s">
+        <v>135</v>
+      </c>
+      <c r="F95" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>100</v>
+      </c>
+      <c r="B96" s="3">
+        <v>2</v>
+      </c>
+      <c r="C96" t="s">
+        <v>114</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="1"/>
+        <v>170-2</v>
+      </c>
+      <c r="E96" t="s">
+        <v>136</v>
+      </c>
+      <c r="F96" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>101</v>
+      </c>
+      <c r="B97" s="3">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
+        <v>114</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="1"/>
+        <v>204-2</v>
+      </c>
+      <c r="E97" t="s">
+        <v>137</v>
+      </c>
+      <c r="F97" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>102</v>
+      </c>
+      <c r="B98" s="3">
+        <v>2</v>
+      </c>
+      <c r="C98" t="s">
+        <v>114</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="1"/>
+        <v>238-2</v>
+      </c>
+      <c r="E98" t="s">
+        <v>138</v>
+      </c>
+      <c r="F98" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>103</v>
+      </c>
+      <c r="B99" s="3">
+        <v>2</v>
+      </c>
+      <c r="C99" t="s">
+        <v>114</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="1"/>
+        <v>272-2</v>
+      </c>
+      <c r="E99" t="s">
+        <v>139</v>
+      </c>
+      <c r="F99" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>104</v>
+      </c>
+      <c r="B100" s="3">
+        <v>2</v>
+      </c>
+      <c r="C100" t="s">
+        <v>114</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="1"/>
+        <v>306-2</v>
+      </c>
+      <c r="E100" t="s">
+        <v>140</v>
+      </c>
+      <c r="F100" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>105</v>
+      </c>
+      <c r="B101" s="3">
+        <v>2</v>
+      </c>
+      <c r="C101" t="s">
+        <v>114</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="1"/>
+        <v>340-2</v>
+      </c>
+      <c r="E101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F101" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>106</v>
+      </c>
+      <c r="B102" s="3">
+        <v>2</v>
+      </c>
+      <c r="C102" t="s">
+        <v>114</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="1"/>
+        <v>408-2</v>
+      </c>
+      <c r="E102" t="s">
+        <v>142</v>
+      </c>
+      <c r="F102" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>107</v>
+      </c>
+      <c r="B103" s="3">
+        <v>3</v>
+      </c>
+      <c r="C103" t="s">
+        <v>115</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="1"/>
+        <v>--3</v>
+      </c>
+      <c r="E103" t="s">
+        <v>108</v>
+      </c>
+      <c r="F103" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>68</v>
+      </c>
+      <c r="B104" s="3">
+        <v>3</v>
+      </c>
+      <c r="C104" t="s">
+        <v>115</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="1"/>
+        <v>S-3</v>
+      </c>
+      <c r="E104" t="s">
+        <v>70</v>
+      </c>
+      <c r="F104" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>69</v>
+      </c>
+      <c r="B105" s="3">
+        <v>3</v>
+      </c>
+      <c r="C105" t="s">
+        <v>115</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="1"/>
+        <v>P-3</v>
+      </c>
+      <c r="E105" t="s">
+        <v>71</v>
+      </c>
+      <c r="F105" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>46</v>
+      </c>
+      <c r="B106" s="3">
+        <v>4</v>
+      </c>
+      <c r="C106" t="s">
+        <v>41</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="1"/>
+        <v>x/x-4</v>
+      </c>
+      <c r="E106" t="s">
+        <v>18</v>
+      </c>
+      <c r="F106" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>47</v>
+      </c>
+      <c r="B107" s="3">
+        <v>4</v>
+      </c>
+      <c r="C107" t="s">
+        <v>41</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="1"/>
+        <v>xR-4</v>
+      </c>
+      <c r="E107" t="s">
+        <v>19</v>
+      </c>
+      <c r="F107" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>10</v>
+      </c>
+      <c r="B108" s="3">
+        <v>5</v>
+      </c>
+      <c r="C108" t="s">
+        <v>42</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="1"/>
+        <v>SS-5</v>
+      </c>
+      <c r="E108" t="s">
+        <v>20</v>
+      </c>
+      <c r="F108" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>11</v>
+      </c>
+      <c r="B109" s="3">
+        <v>5</v>
+      </c>
+      <c r="C109" t="s">
+        <v>42</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="1"/>
+        <v>TN-5</v>
+      </c>
+      <c r="E109" t="s">
+        <v>21</v>
+      </c>
+      <c r="F109" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>12</v>
+      </c>
+      <c r="B110" s="3">
+        <v>5</v>
+      </c>
+      <c r="C110" t="s">
+        <v>42</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="1"/>
+        <v>DK-5</v>
+      </c>
+      <c r="E110" t="s">
+        <v>22</v>
+      </c>
+      <c r="F110" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>13</v>
+      </c>
+      <c r="B111" s="3">
+        <v>5</v>
+      </c>
+      <c r="C111" t="s">
+        <v>42</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="1"/>
+        <v>LG-5</v>
+      </c>
+      <c r="E111" t="s">
+        <v>13</v>
+      </c>
+      <c r="F111" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>107</v>
+      </c>
+      <c r="B112" s="3">
+        <v>6</v>
+      </c>
+      <c r="C112" t="s">
+        <v>43</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="1"/>
+        <v>--6</v>
+      </c>
+      <c r="E112" t="s">
+        <v>109</v>
+      </c>
+      <c r="F112" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>84</v>
+      </c>
+      <c r="B113" s="3">
+        <v>6</v>
+      </c>
+      <c r="C113" t="s">
+        <v>43</v>
+      </c>
+      <c r="D113" t="str">
+        <f t="shared" si="1"/>
+        <v>LL-6</v>
+      </c>
+      <c r="E113" t="s">
+        <v>86</v>
+      </c>
+      <c r="F113" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>85</v>
+      </c>
+      <c r="B114" s="3">
+        <v>6</v>
+      </c>
+      <c r="C114" t="s">
+        <v>43</v>
+      </c>
+      <c r="D114" t="str">
+        <f t="shared" si="1"/>
+        <v>PF-6</v>
+      </c>
+      <c r="E114" t="s">
+        <v>87</v>
+      </c>
+      <c r="F114" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>23</v>
+      </c>
+      <c r="B115" s="3">
+        <v>6</v>
+      </c>
+      <c r="C115" t="s">
+        <v>43</v>
+      </c>
+      <c r="D115" t="str">
+        <f t="shared" si="1"/>
+        <v>EC-6</v>
+      </c>
+      <c r="E115" t="s">
+        <v>25</v>
+      </c>
+      <c r="F115" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>110</v>
+      </c>
+      <c r="B116" s="3">
+        <v>7</v>
+      </c>
+      <c r="C116" t="s">
+        <v>44</v>
+      </c>
+      <c r="D116" t="str">
+        <f t="shared" si="1"/>
+        <v>G4-7</v>
+      </c>
+      <c r="E116" t="s">
+        <v>112</v>
+      </c>
+      <c r="F116" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>111</v>
+      </c>
+      <c r="B117" s="3">
+        <v>7</v>
+      </c>
+      <c r="C117" t="s">
+        <v>44</v>
+      </c>
+      <c r="D117" t="str">
+        <f t="shared" si="1"/>
+        <v>G4+M5 ou G4+F8-7</v>
+      </c>
+      <c r="E117" t="s">
+        <v>113</v>
+      </c>
+      <c r="F117" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>33</v>
+      </c>
+      <c r="B118" s="3">
+        <v>8</v>
+      </c>
+      <c r="C118" t="s">
+        <v>116</v>
+      </c>
+      <c r="D118" t="str">
+        <f t="shared" si="1"/>
+        <v>Acessorios-8</v>
+      </c>
+      <c r="E118" t="s">
+        <v>35</v>
+      </c>
+      <c r="F118" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>34</v>
+      </c>
+      <c r="B119" s="3">
+        <v>9</v>
+      </c>
+      <c r="C119" t="s">
+        <v>45</v>
+      </c>
+      <c r="D119" t="str">
+        <f t="shared" si="1"/>
+        <v>X-9</v>
+      </c>
+      <c r="E119" t="s">
+        <v>37</v>
+      </c>
+      <c r="F119" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>36</v>
+      </c>
+      <c r="B120" s="3">
+        <v>9</v>
+      </c>
+      <c r="C120" t="s">
+        <v>45</v>
+      </c>
+      <c r="D120" t="str">
+        <f t="shared" si="1"/>
+        <v>E -9</v>
+      </c>
+      <c r="E120" t="s">
+        <v>38</v>
+      </c>
+      <c r="F120" t="s">
+        <v>143</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010011CE1B6871DF5745999C1E7BF1D3C675" ma:contentTypeVersion="3" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="4671a090984673c98d9f3d802cfbd84b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c754d3dd-89a9-458c-b6b9-d71350aaa213" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bff7ac9043df59347ee870742dd3d242" ns2:_="">
     <xsd:import namespace="c754d3dd-89a9-458c-b6b9-d71350aaa213"/>
@@ -1114,22 +3461,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FED4FE8-8227-40E8-8088-9DE0F3FBFB99}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB94E07A-902E-4024-9403-0B9E53B2B275}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEBE209C-7BB1-4667-8BA2-62EC8B82B4C7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1145,21 +3494,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB94E07A-902E-4024-9403-0B9E53B2B275}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FED4FE8-8227-40E8-8088-9DE0F3FBFB99}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>